<commit_message>
Updated code - Chaitanya
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data/TEST/KooTestData.XLSX
+++ b/src/main/resources/Test_Data/TEST/KooTestData.XLSX
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\automation\kooframework\src\main\resources\Test_Data\TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\KooApp\src\main\resources\Test_Data\TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A37B824-B5E5-403B-A507-FCED3474AC08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087A79BF-438B-420D-BBA3-70E55846BBDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7550" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVAILABLELANGUAGES" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="1160">
   <si>
     <t>Key</t>
   </si>
@@ -3520,13 +3520,19 @@
   </si>
   <si>
     <t>2. Shared my or someone else's private information.</t>
+  </si>
+  <si>
+    <t>When you add someone to a Favorite, you will see their content and notifications on priority. They will not know that you have added them to your Favorites. It's private.</t>
+  </si>
+  <si>
+    <t>ExplanatoryText</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3538,6 +3544,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3560,7 +3572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3574,6 +3586,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3796,9 +3814,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.08203125" style="4" customWidth="1"/>
     <col min="2" max="16384" width="8.75" style="4"/>
   </cols>
   <sheetData>
@@ -3888,9 +3906,9 @@
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
     <col min="2" max="2" width="45.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3926,7 +3944,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3998,7 +4016,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4078,7 +4096,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -4110,7 +4128,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -4470,7 +4488,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2" ht="28">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -4502,7 +4520,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -4648,7 +4666,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -4763,10 +4781,10 @@
       <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="49.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4801,7 +4819,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4873,7 +4891,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4953,7 +4971,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -4985,7 +5003,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -5345,7 +5363,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -5377,7 +5395,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="28">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -5454,7 +5472,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="56">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -5526,7 +5544,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -5625,9 +5643,9 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
     <col min="2" max="2" width="49.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5663,7 +5681,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5735,7 +5753,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -5815,7 +5833,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -5847,7 +5865,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -6207,7 +6225,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2" ht="28">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -6385,7 +6403,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -6484,7 +6502,7 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
     <col min="2" max="2" width="55.25" style="1" customWidth="1"/>
@@ -6522,7 +6540,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -6594,7 +6612,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -6674,7 +6692,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -6706,7 +6724,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="28">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -7175,7 +7193,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="42.75">
+    <row r="87" spans="1:2" ht="42">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -7353,7 +7371,7 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="35.25" customWidth="1"/>
     <col min="2" max="2" width="42.75" style="1" customWidth="1"/>
@@ -7391,7 +7409,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -7463,7 +7481,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -7543,7 +7561,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -7567,7 +7585,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.5">
+    <row r="27" spans="1:2" ht="28">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -7575,7 +7593,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -8113,7 +8131,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -8212,9 +8230,9 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="42.875" customWidth="1"/>
+    <col min="1" max="1" width="42.83203125" customWidth="1"/>
     <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8250,7 +8268,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -8322,7 +8340,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -8402,7 +8420,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="28">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -8434,7 +8452,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -8972,7 +8990,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="71.25">
+    <row r="96" spans="1:2" ht="70">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -9072,9 +9090,9 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
     <col min="2" max="2" width="46.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9110,7 +9128,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -9182,7 +9200,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -9262,7 +9280,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -9294,7 +9312,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -9760,7 +9778,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="28.5">
+    <row r="87" spans="1:2" ht="28">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -9935,7 +9953,7 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="45.75" customWidth="1"/>
   </cols>
@@ -10025,7 +10043,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="37.25" customWidth="1"/>
@@ -10113,11 +10131,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10199,16 +10217,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="37.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="115.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="115.83203125" style="3" customWidth="1"/>
     <col min="3" max="16384" width="8.75" style="4"/>
   </cols>
   <sheetData>
@@ -10244,7 +10262,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -10852,7 +10870,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.5">
+    <row r="81" spans="1:2">
       <c r="A81" s="4" t="s">
         <v>192</v>
       </c>
@@ -10900,7 +10918,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="56">
       <c r="A87" s="4" t="s">
         <v>204</v>
       </c>
@@ -10972,7 +10990,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -11081,6 +11099,14 @@
       </c>
       <c r="B110" s="3" t="s">
         <v>1157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="28">
+      <c r="A111" s="7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
@@ -11097,10 +11123,10 @@
       <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="37.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.58203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
@@ -11136,7 +11162,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -11208,7 +11234,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -11288,7 +11314,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.5">
+    <row r="24" spans="1:2" ht="28">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -11320,7 +11346,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.5">
+    <row r="28" spans="1:2" ht="28">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -11472,7 +11498,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="28.5">
+    <row r="47" spans="1:2" ht="28">
       <c r="A47" s="1" t="s">
         <v>128</v>
       </c>
@@ -11488,7 +11514,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.5">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>132</v>
       </c>
@@ -11512,7 +11538,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="28.5">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>137</v>
       </c>
@@ -11712,7 +11738,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="28">
       <c r="A77" s="1" t="s">
         <v>184</v>
       </c>
@@ -11744,7 +11770,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="42.75">
+    <row r="81" spans="1:2" ht="42">
       <c r="A81" s="1" t="s">
         <v>192</v>
       </c>
@@ -11789,7 +11815,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="128.25">
+    <row r="87" spans="1:2" ht="112">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -11861,7 +11887,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="42.75">
+    <row r="96" spans="1:2" ht="42">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -11980,7 +12006,7 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="36.75" customWidth="1"/>
     <col min="2" max="2" width="59.75" style="1" customWidth="1"/>
@@ -12018,7 +12044,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -12090,7 +12116,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -12170,7 +12196,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="57">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -12202,7 +12228,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="57">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -12594,7 +12620,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="28">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -12671,7 +12697,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="85.5">
+    <row r="87" spans="1:2" ht="84">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -12743,7 +12769,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -12849,9 +12875,9 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
     <col min="2" max="2" width="100.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12887,7 +12913,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -12959,7 +12985,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -13039,7 +13065,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -13463,7 +13489,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="28">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -13540,7 +13566,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="56">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -13714,9 +13740,9 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.58203125" customWidth="1"/>
     <col min="2" max="2" width="59.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.75" customWidth="1"/>
   </cols>
@@ -13753,7 +13779,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -13825,7 +13851,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="28">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -13905,7 +13931,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="42">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -13937,7 +13963,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="42">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -14329,7 +14355,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="28">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -14406,7 +14432,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="71.25">
+    <row r="87" spans="1:2" ht="70">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -14478,7 +14504,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="28">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>

</xml_diff>

<commit_message>
Updated Code - D Jagath chandra
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data/TEST/KooTestData.XLSX
+++ b/src/main/resources/Test_Data/TEST/KooTestData.XLSX
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\automation\kooframework\src\main\resources\Test_Data\TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\KooApp\src\main\resources\Test_Data\TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A37B824-B5E5-403B-A507-FCED3474AC08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C8C8BE-2282-43E7-8B4A-0C706F84ED7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVAILABLELANGUAGES" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="1226">
   <si>
     <t>Key</t>
   </si>
@@ -3520,13 +3520,217 @@
   </si>
   <si>
     <t>2. Shared my or someone else's private information.</t>
+  </si>
+  <si>
+    <t>ReportUserOption1Txt</t>
+  </si>
+  <si>
+    <t>ReportUserOption2Txt</t>
+  </si>
+  <si>
+    <t>ReportUserOption3Txt</t>
+  </si>
+  <si>
+    <t>3. Spam, Scam or Phishing</t>
+  </si>
+  <si>
+    <t>ReportUserOption4Txt</t>
+  </si>
+  <si>
+    <t>4. Intellectual Property Infringement</t>
+  </si>
+  <si>
+    <t>ReportUserOption5Txt</t>
+  </si>
+  <si>
+    <t>5. Self Injury or Suicide</t>
+  </si>
+  <si>
+    <t>ReportUserOption6Txt</t>
+  </si>
+  <si>
+    <t>6. Conducts Illegal Activities</t>
+  </si>
+  <si>
+    <t>ReportUserOption7Txt</t>
+  </si>
+  <si>
+    <t>7. Pretending to be me or someone else</t>
+  </si>
+  <si>
+    <t>ReportUserOption8Txt</t>
+  </si>
+  <si>
+    <t>8. Something Else</t>
+  </si>
+  <si>
+    <t>ReportUserOption9Txt</t>
+  </si>
+  <si>
+    <t>9. Not Interested/ Not Relevant</t>
+  </si>
+  <si>
+    <t>ReportKooOption1Txt</t>
+  </si>
+  <si>
+    <t>1. Hate Speech and Discrimination</t>
+  </si>
+  <si>
+    <t>ReportKooOption2Txt</t>
+  </si>
+  <si>
+    <t>2. Religiously Offensive Content</t>
+  </si>
+  <si>
+    <t>ReportKooOption3Txt</t>
+  </si>
+  <si>
+    <t>3. Terrorism and Extremism</t>
+  </si>
+  <si>
+    <t>ReportKooOption4Txt</t>
+  </si>
+  <si>
+    <t>4. Dangerous, Violent Content (Death or Injury)</t>
+  </si>
+  <si>
+    <t>ReportKooOption5Txt</t>
+  </si>
+  <si>
+    <t>5. Graphic, Obscene or Sexual Content</t>
+  </si>
+  <si>
+    <t>ReportKooOption6Txt</t>
+  </si>
+  <si>
+    <t>6. Provoking Koo / Comment</t>
+  </si>
+  <si>
+    <t>ReportKooOption7Txt</t>
+  </si>
+  <si>
+    <t>7. Misinformation and Disinformation</t>
+  </si>
+  <si>
+    <t>ReportKooOption8Txt</t>
+  </si>
+  <si>
+    <t>8. Malicious Programmes, URL or Code</t>
+  </si>
+  <si>
+    <t>ReportKooOption9Txt</t>
+  </si>
+  <si>
+    <t>9. Child Abuse</t>
+  </si>
+  <si>
+    <t>ReportKooOption10Txt</t>
+  </si>
+  <si>
+    <t>10. Not Interested/ Not Relevant</t>
+  </si>
+  <si>
+    <t>OnBoardingPage1HeaderText</t>
+  </si>
+  <si>
+    <t>Add your name</t>
+  </si>
+  <si>
+    <t>OnBoardingPage2HeaderText</t>
+  </si>
+  <si>
+    <t>Add Profile Picture</t>
+  </si>
+  <si>
+    <t>OnBoardingPage3HeaderText</t>
+  </si>
+  <si>
+    <t>Your Preferences</t>
+  </si>
+  <si>
+    <t>OnBoardingPage4HeaderText</t>
+  </si>
+  <si>
+    <t>OnBoardingPage5HeaderText</t>
+  </si>
+  <si>
+    <t>Follow Topics</t>
+  </si>
+  <si>
+    <t>AccountSectionOption1Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption2Text</t>
+  </si>
+  <si>
+    <t>Account Information</t>
+  </si>
+  <si>
+    <t>AccountSectionOption3Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption4Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption5Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption6Text</t>
+  </si>
+  <si>
+    <t>Manage Subscriptions</t>
+  </si>
+  <si>
+    <t>AccountSectionOption7Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption8Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption9Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption10Text</t>
+  </si>
+  <si>
+    <t>AccountSectionOption11Text</t>
+  </si>
+  <si>
+    <t>Add Account</t>
+  </si>
+  <si>
+    <t>AccountSectionOption12Text</t>
+  </si>
+  <si>
+    <t>SearchAllResultTabs1</t>
+  </si>
+  <si>
+    <t>SearchAllResultTabs2</t>
+  </si>
+  <si>
+    <t>SearchAllResultTabs3</t>
+  </si>
+  <si>
+    <t>Hashtags</t>
+  </si>
+  <si>
+    <t>SearchAllResultTabs4</t>
+  </si>
+  <si>
+    <t>Koos</t>
+  </si>
+  <si>
+    <t>AccountSectionOption1TextById</t>
+  </si>
+  <si>
+    <t>AccountSectionOption2TextById</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3538,6 +3742,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3560,7 +3770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3574,6 +3784,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3796,10 +4012,10 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="8.75" style="4"/>
+    <col min="1" max="1" width="10.09765625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="8.69921875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3888,10 +4104,10 @@
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="45.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
+    <col min="2" max="2" width="45.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3926,7 +4142,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3998,7 +4214,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4078,7 +4294,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -4110,7 +4326,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -4470,7 +4686,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2" ht="27.6">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -4502,7 +4718,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -4648,7 +4864,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -4763,10 +4979,10 @@
       <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="49.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
+    <col min="2" max="2" width="49.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4801,7 +5017,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4873,7 +5089,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4953,7 +5169,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -4985,7 +5201,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -5345,7 +5561,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -5377,7 +5593,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -5454,7 +5670,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="55.2">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -5526,7 +5742,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -5625,10 +5841,10 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="49.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
+    <col min="2" max="2" width="49.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5663,7 +5879,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5735,7 +5951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -5815,7 +6031,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -5847,7 +6063,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -6207,7 +6423,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="28.5">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>176</v>
       </c>
@@ -6385,7 +6601,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -6484,10 +6700,10 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
-    <col min="2" max="2" width="55.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6522,7 +6738,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -6594,7 +6810,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -6674,7 +6890,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -6706,7 +6922,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="27.6">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -7175,7 +7391,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="42.75">
+    <row r="87" spans="1:2" ht="41.4">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -7353,10 +7569,10 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="35.25" customWidth="1"/>
-    <col min="2" max="2" width="42.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.19921875" customWidth="1"/>
+    <col min="2" max="2" width="42.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -7391,7 +7607,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -7463,7 +7679,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -7543,7 +7759,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -7567,7 +7783,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.5">
+    <row r="27" spans="1:2" ht="27.6">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -7575,7 +7791,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -8113,7 +8329,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -8212,9 +8428,9 @@
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="42.875" customWidth="1"/>
+    <col min="1" max="1" width="42.8984375" customWidth="1"/>
     <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8250,7 +8466,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -8322,7 +8538,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -8402,7 +8618,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -8434,7 +8650,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -8972,7 +9188,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="71.25">
+    <row r="96" spans="1:2" ht="69">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -9072,10 +9288,10 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="46.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
+    <col min="2" max="2" width="46.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9110,7 +9326,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -9182,7 +9398,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -9262,7 +9478,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -9294,7 +9510,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -9760,7 +9976,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="28.5">
+    <row r="87" spans="1:2" ht="27.6">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -9935,9 +10151,9 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="45.75" customWidth="1"/>
+    <col min="2" max="2" width="45.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10025,10 +10241,10 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="37.25" customWidth="1"/>
+    <col min="2" max="2" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10113,11 +10329,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -10199,17 +10415,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="37.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="115.875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="8.75" style="4"/>
+    <col min="1" max="1" width="37.8984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="115.8984375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.69921875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10244,7 +10460,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -10852,7 +11068,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="28.5">
+    <row r="81" spans="1:2">
       <c r="A81" s="4" t="s">
         <v>192</v>
       </c>
@@ -10900,7 +11116,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="55.2">
       <c r="A87" s="4" t="s">
         <v>204</v>
       </c>
@@ -10972,7 +11188,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -11069,7 +11285,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="4" t="s">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>1155</v>
@@ -11077,10 +11293,330 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="4" t="s">
-        <v>1156</v>
+        <v>1159</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>1157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="4" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="4" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="6" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="6" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="6" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="6" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="6" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="6" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="6" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="6" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="6" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="6" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="6" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="4" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>1223</v>
       </c>
     </row>
   </sheetData>
@@ -11097,11 +11633,11 @@
       <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="37.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="37.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.59765625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -11136,7 +11672,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -11208,7 +11744,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -11288,7 +11824,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.5">
+    <row r="24" spans="1:2" ht="27.6">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -11320,7 +11856,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.5">
+    <row r="28" spans="1:2" ht="27.6">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -11472,7 +12008,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="28.5">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>128</v>
       </c>
@@ -11488,7 +12024,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.5">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>132</v>
       </c>
@@ -11512,7 +12048,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="28.5">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>137</v>
       </c>
@@ -11712,7 +12248,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="27.6">
       <c r="A77" s="1" t="s">
         <v>184</v>
       </c>
@@ -11744,7 +12280,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="42.75">
+    <row r="81" spans="1:2" ht="41.4">
       <c r="A81" s="1" t="s">
         <v>192</v>
       </c>
@@ -11789,7 +12325,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="128.25">
+    <row r="87" spans="1:2" ht="110.4">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -11861,7 +12397,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="42.75">
+    <row r="96" spans="1:2" ht="41.4">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -11980,10 +12516,10 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="36.75" customWidth="1"/>
-    <col min="2" max="2" width="59.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.69921875" customWidth="1"/>
+    <col min="2" max="2" width="59.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -12018,7 +12554,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -12090,7 +12626,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -12170,7 +12706,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="57">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -12202,7 +12738,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="57">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -12594,7 +13130,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="27.6">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -12671,7 +13207,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="85.5">
+    <row r="87" spans="1:2" ht="82.8">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -12743,7 +13279,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -12798,7 +13334,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="10.9" customHeight="1">
+    <row r="104" spans="1:2" ht="10.95" customHeight="1">
       <c r="A104" s="4" t="s">
         <v>231</v>
       </c>
@@ -12849,9 +13385,9 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
     <col min="2" max="2" width="100.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12887,7 +13423,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -12959,7 +13495,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -13039,7 +13575,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="27.6">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -13463,7 +13999,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -13540,7 +14076,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="57">
+    <row r="87" spans="1:2" ht="55.2">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -13714,11 +14250,11 @@
       <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="59.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" customWidth="1"/>
+    <col min="2" max="2" width="59.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13753,7 +14289,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5">
+    <row r="5" spans="1:2" ht="27.6">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -13825,7 +14361,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5">
+    <row r="14" spans="1:2" ht="27.6">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -13905,7 +14441,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75">
+    <row r="24" spans="1:2" ht="41.4">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -13937,7 +14473,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="42.75">
+    <row r="28" spans="1:2" ht="41.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -14329,7 +14865,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="28.5">
+    <row r="77" spans="1:2" ht="27.6">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -14406,7 +14942,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="71.25">
+    <row r="87" spans="1:2" ht="69">
       <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
@@ -14478,7 +15014,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="28.5">
+    <row r="96" spans="1:2" ht="27.6">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>

</xml_diff>

<commit_message>
Test data sheet updated
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data/TEST/KooTestData.XLSX
+++ b/src/main/resources/Test_Data/TEST/KooTestData.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\KooApp\src\main\resources\Test_Data\TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087A79BF-438B-420D-BBA3-70E55846BBDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A42B3A1-86BD-40A5-83A9-0B2AF77EE7EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7550" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,11 +31,12 @@
     <sheet name="Portuguese" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="1164">
   <si>
     <t>Key</t>
   </si>
@@ -3526,6 +3527,18 @@
   </si>
   <si>
     <t>ExplanatoryText</t>
+  </si>
+  <si>
+    <t>HomePageTabsNoOnBoardingSelection</t>
+  </si>
+  <si>
+    <t>Feed,People,Topics</t>
+  </si>
+  <si>
+    <t>HomePageTabsNotPresentWhenNoOnBoardingSelection</t>
+  </si>
+  <si>
+    <t>Polls,Videos,Friends,New,Following,Popular</t>
   </si>
 </sst>
 </file>
@@ -10217,10 +10230,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14"/>
@@ -11101,11 +11114,27 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="28">
-      <c r="A111" s="7" t="s">
+    <row r="111" spans="1:2">
+      <c r="A111" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="28">
+      <c r="A113" s="7" t="s">
         <v>1159</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="B113" s="6" t="s">
         <v>1158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code Search and Settings Pages
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data/TEST/KooTestData.XLSX
+++ b/src/main/resources/Test_Data/TEST/KooTestData.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\KooApp\src\main\resources\Test_Data\TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C8C8BE-2282-43E7-8B4A-0C706F84ED7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217CD32E-A920-4B33-8640-F4CC1E3C502C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="1231">
   <si>
     <t>Key</t>
   </si>
@@ -3724,6 +3724,21 @@
   </si>
   <si>
     <t>AccountSectionOption2TextById</t>
+  </si>
+  <si>
+    <t>AccountsSectionAccountInformationSubHeading</t>
+  </si>
+  <si>
+    <t>AccountsSectionSuperLikesSubHeading</t>
+  </si>
+  <si>
+    <t>Super Likes</t>
+  </si>
+  <si>
+    <t>AccountsSectionManageSubscriptionsSubHeading</t>
+  </si>
+  <si>
+    <t>AccountsSectionManageBlockedUsersSubHeading</t>
   </si>
 </sst>
 </file>
@@ -10415,15 +10430,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B150"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="37.8984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="42.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="115.8984375" style="3" customWidth="1"/>
     <col min="3" max="16384" width="8.69921875" style="4"/>
   </cols>
@@ -10782,840 +10797,872 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>124</v>
+        <v>1226</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>125</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
-        <v>132</v>
+        <v>1227</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>133</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="4" t="s">
-        <v>134</v>
+        <v>1229</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>135</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
-        <v>136</v>
+        <v>1230</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>144</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="4" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="4" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="4" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="4" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="55.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="4" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="55.2">
       <c r="A91" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>93</v>
+        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="4" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="27.6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>225</v>
+        <v>121</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>218</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="27.6">
       <c r="A100" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>189</v>
+        <v>224</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>67</v>
+      <c r="A106" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>236</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>27</v>
+        <v>232</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="4" t="s">
-        <v>1158</v>
+        <v>233</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="4" t="s">
-        <v>1159</v>
+      <c r="A110" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1157</v>
+        <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="4" t="s">
-        <v>1160</v>
+        <v>235</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1161</v>
+        <v>236</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="4" t="s">
-        <v>1162</v>
+        <v>237</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1163</v>
+        <v>27</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="4" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1165</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="4" t="s">
-        <v>1166</v>
+        <v>1159</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1167</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="4" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="4" t="s">
-        <v>1170</v>
+        <v>1162</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="4" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="4" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="4" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="4" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="4" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="4" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="4" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="4" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="4" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="4" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="4" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="4" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="4" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="4" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="4" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>189</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="4" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="4" t="s">
         <v>1201</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B136" s="3" t="s">
         <v>1202</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="6" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="6" t="s">
-        <v>1204</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="6" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="6" t="s">
-        <v>1207</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="6" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>129</v>
+        <v>1203</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="6" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="6" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="6" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="6" t="s">
-        <v>1213</v>
+        <v>1208</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="6" t="s">
-        <v>1214</v>
+        <v>1209</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>135</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="6" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="6" t="s">
-        <v>1217</v>
+        <v>1212</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="6" t="s">
-        <v>1224</v>
+        <v>1213</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>1216</v>
+        <v>133</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="6" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="6" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="6" t="s">
         <v>1225</v>
       </c>
-      <c r="B146" s="7" t="s">
+      <c r="B150" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="4" t="s">
+    <row r="151" spans="1:2">
+      <c r="A151" s="4" t="s">
         <v>1218</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B151" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="4" t="s">
+    <row r="152" spans="1:2">
+      <c r="A152" s="4" t="s">
         <v>1219</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B152" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="4" t="s">
+    <row r="153" spans="1:2">
+      <c r="A153" s="4" t="s">
         <v>1220</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>1221</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="4" t="s">
+    <row r="154" spans="1:2">
+      <c r="A154" s="4" t="s">
         <v>1222</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B154" s="3" t="s">
         <v>1223</v>
       </c>
     </row>

</xml_diff>